<commit_message>
update ex file for easier parsing
</commit_message>
<xml_diff>
--- a/assets/example_files/report_scraper_ex.xlsx
+++ b/assets/example_files/report_scraper_ex.xlsx
@@ -43,7 +43,7 @@
     <t>OCT 2024</t>
   </si>
   <si>
-    <t>fishing-reports|report</t>
+    <t>fishing-reports, report</t>
   </si>
   <si>
     <t>news</t>
@@ -64,7 +64,7 @@
     <t>https://www.thetackleshop.com/</t>
   </si>
   <si>
-    <t>montana-fly-fishing-reports|fishing-report|fishing_report</t>
+    <t>montana-fly-fishing-reports, fishing-report</t>
   </si>
   <si>
     <t>page</t>
@@ -76,10 +76,10 @@
     <t>APR 2025</t>
   </si>
   <si>
-    <t>fishing-reports|post</t>
-  </si>
-  <si>
-    <t>news|tags|hashtags</t>
+    <t>fishing-reports, post</t>
+  </si>
+  <si>
+    <t>news, tags, hashtags</t>
   </si>
   <si>
     <t>https://snakeriverangler.com/</t>
@@ -88,7 +88,7 @@
     <t>article:not(:has(a:text-matches("read more", "i")))</t>
   </si>
   <si>
-    <t>fishing-reports|fishing-report</t>
+    <t>fishing-reports, fishing-report</t>
   </si>
   <si>
     <t>READ MORE</t>
@@ -97,10 +97,10 @@
     <t>http://worldcastanglers.com/</t>
   </si>
   <si>
-    <t>jackson-hole-fishing-report|fishing-report</t>
-  </si>
-  <si>
-    <t>trip-report|tag</t>
+    <t>jackson-hole-fishing-report, fishing-report</t>
+  </si>
+  <si>
+    <t>trip-report, tag</t>
   </si>
   <si>
     <t>Read more</t>
@@ -109,7 +109,7 @@
     <t>http://www.montanaangler.com/</t>
   </si>
   <si>
-    <t>montana-fishing-reports|montana-fishing-report</t>
+    <t>montana-fishing-reports, montana-fishing-report</t>
   </si>
   <si>
     <t>Read More</t>
@@ -139,13 +139,13 @@
     <t>https://bighornangler.com/</t>
   </si>
   <si>
-    <t>reports|fishing-report</t>
+    <t>reports, fishing-report</t>
   </si>
   <si>
     <t>http://trroutfitters.com/</t>
   </si>
   <si>
-    <t>uploads|page</t>
+    <t>uploads, page</t>
   </si>
   <si>
     <t>https://www.beartoothflyfishing.com/</t>
@@ -154,10 +154,10 @@
     <t>div.post</t>
   </si>
   <si>
-    <t>fishing-reports-tips|fishing-reports|fishing-report</t>
-  </si>
-  <si>
-    <t>page|tag</t>
+    <t>fishing-reports-tips, fishing-reports, fishing-report</t>
+  </si>
+  <si>
+    <t>page, tag</t>
   </si>
   <si>
     <t>http://www.sweetwaterflyshop.com/</t>
@@ -187,7 +187,7 @@
     <t>div.reportContent</t>
   </si>
   <si>
-    <t>fishing-report|fishing-reports</t>
+    <t>fishing-report, fishing-reports</t>
   </si>
   <si>
     <t>http://blackfootriver.com/</t>
@@ -205,7 +205,7 @@
     <t>2025</t>
   </si>
   <si>
-    <t>fishing-reports|fishing_report</t>
+    <t>fishing-reports, fishing_report</t>
   </si>
   <si>
     <t>View Report</t>
@@ -235,7 +235,7 @@
     <t>div._1140-w-wrapper:has(h1:text-matches("fishing report", "i"))</t>
   </si>
   <si>
-    <t>fishing-report|river-report</t>
+    <t>fishing-report, river-report</t>
   </si>
   <si>
     <t>https://theriversedge.com/</t>
@@ -244,7 +244,7 @@
     <t>div.container:has(h2:text-matches("river fishing report", "i"))</t>
   </si>
   <si>
-    <t>montana-fishing-reports|fishing-report</t>
+    <t>montana-fishing-reports, fishing-report</t>
   </si>
   <si>
     <t>View recent fishing reports</t>
@@ -256,7 +256,7 @@
     <t>div.mb-5:has(h2:text-matches("Fly Pattern Suggestions", "i"))</t>
   </si>
   <si>
-    <t>river-reports|reports</t>
+    <t>river-reports, reports</t>
   </si>
   <si>
     <t>http://madisonriveroutfitters.com/</t>
@@ -265,7 +265,7 @@
     <t>div.container.main.content</t>
   </si>
   <si>
-    <t>madison-river-fishing-reports|fly-fishing-report</t>
+    <t>madison-river-fishing-reports, fly-fishing-report</t>
   </si>
   <si>
     <t>https://www.thestonefly.com/</t>

</xml_diff>